<commit_message>
Added new Extracted Tweets
</commit_message>
<xml_diff>
--- a/ExcelSheets/15-Date.xlsx
+++ b/ExcelSheets/15-Date.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\twitterAnalyze\TweetsAnalyze\ExcelSheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\twitterAnalyze\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="20490" windowHeight="7890"/>
+    <workbookView xWindow="0" yWindow="900" windowWidth="20490" windowHeight="7890"/>
   </bookViews>
   <sheets>
     <sheet name="Days" sheetId="1" r:id="rId1"/>
@@ -1875,8 +1875,13 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{41D2F452-3C0C-402C-8745-039A1DA62087}">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{147A421F-539F-43B2-BB0B-82725F5570DD}" diskRevisions="1" revisionId="1" version="2">
   <header guid="{41D2F452-3C0C-402C-8745-039A1DA62087}" dateTime="2016-08-15T12:55:44" maxSheetId="2" userName="Rushabh Wadkar" r:id="rId1">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{147A421F-539F-43B2-BB0B-82725F5570DD}" dateTime="2016-08-15T12:59:12" maxSheetId="2" userName="Rushabh Wadkar" r:id="rId2" minRId="1">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
@@ -1888,7 +1893,20 @@
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
 </file>
 
-<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1" sId="1" numFmtId="4">
+    <oc r="O14">
+      <v>0.90588575601577759</v>
+    </oc>
+    <nc r="O14">
+      <v>0.8</v>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
 <users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="0"/>
 </file>
 
@@ -2157,7 +2175,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P251"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -2744,7 +2764,7 @@
         <v>35</v>
       </c>
       <c r="O14" s="2">
-        <v>0.90588575601577759</v>
+        <v>0.8</v>
       </c>
       <c r="P14" s="2">
         <v>0.99370269900966068</v>

</xml_diff>